<commit_message>
added isosteric heat calculation
</commit_message>
<xml_diff>
--- a/tests/calculations/data/isotherms/BAX 1500 - Isosteric Heat - 298.xlsx
+++ b/tests/calculations/data/isotherms/BAX 1500 - Isosteric Heat - 298.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="11" documentId="126F6F5A08F7605938CC69D5F77355AE475FF44B" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{BBE32C5F-F591-41B1-8E21-0E743BE494CF}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="126F6F5A08F7605938CC69D5F77355AE475FF44B" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{7E2C979D-5BF1-4391-8E61-24C168C154F9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,13 +116,13 @@
     <t>C_m</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>C4H10</t>
   </si>
   <si>
-    <t>BAX 1500</t>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>TB</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +623,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>298.14999999999998</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -665,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>